<commit_message>
Fix item and solve #53
</commit_message>
<xml_diff>
--- a/inst/formr/bvq-1.0.1/bvq_grammar.xlsx
+++ b/inst/formr/bvq-1.0.1/bvq_grammar.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Documents\software\bvq\inst\formr\bvq-1.0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggarciad\OneDrive - San Juan de Dios\Documentos\projects\bvq\inst\formr\bvq-1.0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EDC2CD-F49F-4F52-A4AB-9D9EBF6FD8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="-16320" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -748,16 +747,16 @@
     <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("**Quants minuts a la setmana li llegiu contes curts o històries (amb dibuixos)?**"), bvq_01_log$language == "spanish" ~paste0("**¿Cuántos minutos a la semana le léeis cuentos cortos / historias (con dibujos) a vuestro hijo?**"), TRUE ~ paste0("**How many minutes per week do you read stories (with illustrations) to your child?**")))`</t>
   </si>
   <si>
-    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Moltes flor"), bvq_01_log$language == "spanish" ~paste0("Muchs flor"), TRUE ~ paste0("Lot flowers")))`</t>
-  </si>
-  <si>
     <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Molts cotxe"), bvq_01_log$language == "spanish" ~paste0("Muchos coche"), TRUE ~ paste0("Lot car")))`</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Moltes flor"), bvq_01_log$language == "spanish" ~paste0("Muchas flor"), TRUE ~ paste0("Lot flowers")))`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
@@ -1029,24 +1028,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="20" style="1" customWidth="1"/>
-    <col min="3" max="3" width="30" style="1" customWidth="1"/>
-    <col min="4" max="4" width="46.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46.08203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="1"/>
     <col min="6" max="6" width="81" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1075,7 +1074,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" customFormat="1" ht="380" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" customFormat="1" ht="384.75" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1113,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" customFormat="1" ht="280" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" customFormat="1" ht="283.5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1130,7 +1129,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" customFormat="1" ht="260" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" customFormat="1" ht="263.25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1147,7 +1146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" customFormat="1" ht="100" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" customFormat="1" ht="101.25" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1164,7 +1163,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1232,7 +1231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9" customFormat="1" ht="60" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" customFormat="1" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1266,7 +1265,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -1284,7 +1283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" customFormat="1" ht="40" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1299,7 +1298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:9" customFormat="1" ht="40" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" customFormat="1" ht="40" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1329,7 +1328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:9" customFormat="1" ht="40" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:9" customFormat="1" ht="40" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -1359,7 +1358,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" customFormat="1" ht="40" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" customFormat="1" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -1374,7 +1373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -1395,19 +1394,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="20" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>50</v>
       </c>
@@ -1418,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -1429,7 +1428,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1440,7 +1439,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1462,7 +1461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1473,7 +1472,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1484,7 +1483,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>66</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -1506,7 +1505,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1528,7 +1527,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1539,7 +1538,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1558,10 +1557,10 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>75</v>
       </c>
@@ -1572,7 +1571,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -1580,10 +1579,10 @@
         <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -1601,16 +1600,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="20" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>79</v>
       </c>
@@ -1618,7 +1617,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1626,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1634,7 +1633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1642,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -1650,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -1658,12 +1657,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>87</v>
       </c>
@@ -1679,7 +1678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -1687,7 +1686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -1695,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>90</v>
       </c>

</xml_diff>